<commit_message>
create V0.2 with csv upload to handle issue on shinyapps.io
</commit_message>
<xml_diff>
--- a/Input_Excel_Example.xlsx
+++ b/Input_Excel_Example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3fdf6d9f7afe5b85/Dokumente/Projects/CookiePlanner/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3fdf6d9f7afe5b85/Dokumente/GitHub/CookiePlanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{CC1EB012-5510-4942-BB14-3578F046B2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D8CE728-1CEB-4D9E-B981-C1015FD8B6F9}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{CC1EB012-5510-4942-BB14-3578F046B2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9F8752F-A5C2-4927-AA7E-1031B3B79ED4}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{94744077-A3A9-4F9A-B4E7-4B080947AE13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{94744077-A3A9-4F9A-B4E7-4B080947AE13}"/>
   </bookViews>
   <sheets>
     <sheet name="Recipes" sheetId="1" r:id="rId1"/>
@@ -512,7 +512,7 @@
   <dimension ref="A1:AG501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -670,9 +670,7 @@
       <c r="F2" s="1">
         <v>4</v>
       </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="1">
         <v>200</v>
       </c>

</xml_diff>

<commit_message>
Create version 0.3 with new features and change UI
New features:
- Supports floats as recipe quantities
- Guesses delimiter of csv
- Multiplier column not included anymore
- fixed header of input/output table
- fixed first column of input (recipe name)
- minor UI improvements
</commit_message>
<xml_diff>
--- a/Input_Excel_Example.xlsx
+++ b/Input_Excel_Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3fdf6d9f7afe5b85/Dokumente/GitHub/CookiePlanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{CC1EB012-5510-4942-BB14-3578F046B2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBAF4A9D-CBA7-46AB-BDD0-4785A4ECE262}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="8_{CC1EB012-5510-4942-BB14-3578F046B2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7A499C3-2D3A-4B2C-848C-5FE876AB3BFA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{94744077-A3A9-4F9A-B4E7-4B080947AE13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{94744077-A3A9-4F9A-B4E7-4B080947AE13}"/>
   </bookViews>
   <sheets>
     <sheet name="Explanation" sheetId="5" r:id="rId1"/>
@@ -685,7 +685,7 @@
   </sheetPr>
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -766,8 +766,8 @@
   </sheetPr>
   <dimension ref="A1:AG501"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -930,7 +930,7 @@
         <v>200</v>
       </c>
       <c r="I2" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>

</xml_diff>